<commit_message>
fixed negative comment scores
</commit_message>
<xml_diff>
--- a/feature_analysis/Jupiter Notebooks/y_vals.xlsx
+++ b/feature_analysis/Jupiter Notebooks/y_vals.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -495,7 +495,7 @@
         <v>73758</v>
       </c>
       <c r="B3" t="n">
-        <v>0.001949317738791423</v>
+        <v>0.00186046511627907</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -509,7 +509,7 @@
         <v>1024</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="G3" t="n">
         <v>2</v>
@@ -520,7 +520,7 @@
         <v>88611</v>
       </c>
       <c r="B4" t="n">
-        <v>0.9443005181347151</v>
+        <v>0.9448717948717948</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -537,7 +537,7 @@
         <v>41</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
@@ -545,7 +545,7 @@
         <v>93218</v>
       </c>
       <c r="B5" t="n">
-        <v>0.01176470588235294</v>
+        <v>0.01162790697674419</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -559,7 +559,7 @@
         <v>163</v>
       </c>
       <c r="F5" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -584,7 +584,7 @@
         <v>69</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -670,7 +670,7 @@
         <v>173147</v>
       </c>
       <c r="B10" t="n">
-        <v>0.9848942598187311</v>
+        <v>0.9850746268656716</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -678,7 +678,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="E10" t="n">
         <v>1</v>
@@ -687,7 +687,7 @@
         <v>9</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
@@ -853,7 +853,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>542</v>
+        <v>582</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -862,7 +862,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18">

</xml_diff>